<commit_message>
Update cpl for usb resistors
</commit_message>
<xml_diff>
--- a/mippe_base_32u4/CPL_REV_A.xlsx
+++ b/mippe_base_32u4/CPL_REV_A.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t xml:space="preserve">32.2mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.75mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15mm</t>
   </si>
   <si>
     <t xml:space="preserve">R7</t>
@@ -266,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,7 +489,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -488,10 +500,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
@@ -511,28 +523,48 @@
         <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
@@ -569,8 +601,20 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>